<commit_message>
Update Times spreadsheet with complete data
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -121,7 +121,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -145,14 +145,14 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="A2:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -172,10 +172,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>306</v>
+        <v>200</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>401</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,10 +183,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>756</v>
+        <v>603</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>971</v>
+        <v>890</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -194,10 +194,10 @@
         <v>50</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>2574</v>
+        <v>2633</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>2524</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,10 +205,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>7571</v>
+        <v>8234</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>6095</v>
+        <v>6488</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,10 +216,10 @@
         <v>200</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>21577</v>
+        <v>28163</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>13102</v>
+        <v>14408</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,10 +227,10 @@
         <v>500</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>107831</v>
+        <v>159230</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>36301</v>
+        <v>41229</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,10 +238,10 @@
         <v>1000</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>399593</v>
+        <v>520348</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>80120</v>
+        <v>93065</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,10 +249,10 @@
         <v>2000</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>1883061</v>
+        <v>2426939</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>173347</v>
+        <v>200020</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,10 +260,10 @@
         <v>5000</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>11489047</v>
+        <v>15060753</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>480777</v>
+        <v>557087</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -271,10 +271,10 @@
         <v>10000</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>46225172</v>
+        <v>60196776</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1048128</v>
+        <v>1202024</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,10 +282,10 @@
         <v>20000</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>185479504</v>
+        <v>241359648</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>2278419</v>
+        <v>2592190</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,10 +293,10 @@
         <v>50000</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>1141171456</v>
+        <v>1510104320</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>6023497</v>
+        <v>7134107</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,10 +304,10 @@
         <v>100000</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>4562833920</v>
+        <v>6052056064</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>13038048</v>
+        <v>15452036</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,20 +315,32 @@
         <v>200000</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>18411907072</v>
+        <v>24300070912</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>28481332</v>
+        <v>33289444</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>500000</v>
       </c>
+      <c r="B16" s="1" t="n">
+        <v>151931191296</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>91971272</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>1000000</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>608352927744</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>195395824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>